<commit_message>
Updated Progress Report and SRS
SRS - added a few acceptance criteria on US 3
</commit_message>
<xml_diff>
--- a/Progress-Report.xlsx
+++ b/Progress-Report.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12320" yWindow="1400" windowWidth="23860" windowHeight="17540" activeTab="2"/>
+    <workbookView xWindow="6820" yWindow="500" windowWidth="23860" windowHeight="17540" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="User Interface" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
   <si>
     <t>DONE</t>
   </si>
@@ -896,7 +896,7 @@
   <dimension ref="B1:G29"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -957,7 +957,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="D4" s="6">
         <f>--(Table14[[#This Row],[% COMPLETE]]&gt;=1)</f>
@@ -1186,8 +1186,8 @@
   </sheetPr>
   <dimension ref="B1:H21"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1488,11 +1488,11 @@
         <v>1</v>
       </c>
       <c r="E17" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="9">
         <f>--(Table1[[#This Row],[% COMPLETE]]&gt;=1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="1" t="s">
@@ -1564,11 +1564,11 @@
         <v>1</v>
       </c>
       <c r="E21" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" s="9">
         <f>--(Table1[[#This Row],[% COMPLETE]]&gt;=1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="1" t="s">
@@ -1657,8 +1657,8 @@
   </sheetPr>
   <dimension ref="B1:G21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1980,13 +1980,15 @@
         <v>1</v>
       </c>
       <c r="D20" s="22">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E20" s="17">
         <f>--(Table13[[#This Row],[% COMPLETE]]&gt;=1)</f>
         <v>0</v>
       </c>
-      <c r="F20" s="2"/>
+      <c r="F20" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="G20" s="4" t="s">
         <v>45</v>
       </c>
@@ -2094,7 +2096,7 @@
   </sheetPr>
   <dimension ref="B1:G13"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Uploaded CD and updated PR
Class diagram for iteration 1
</commit_message>
<xml_diff>
--- a/Progress-Report.xlsx
+++ b/Progress-Report.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6820" yWindow="500" windowWidth="23860" windowHeight="17540" activeTab="3"/>
+    <workbookView xWindow="6820" yWindow="500" windowWidth="23860" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="User Interface" sheetId="5" r:id="rId1"/>
@@ -62,18 +62,12 @@
     <t>Software System Specficiation</t>
   </si>
   <si>
-    <t>Class Diagram</t>
-  </si>
-  <si>
     <t>Entity-Relationship Model</t>
   </si>
   <si>
     <t>Project Plan</t>
   </si>
   <si>
-    <t>To be done during Integration II</t>
-  </si>
-  <si>
     <t>Login / Register</t>
   </si>
   <si>
@@ -189,6 +183,12 @@
   </si>
   <si>
     <t>Still to test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iteration 1 Class Diagram </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iteration 2 Class Diagram </t>
   </si>
 </sst>
 </file>
@@ -895,8 +895,8 @@
   </sheetPr>
   <dimension ref="B1:G29"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -933,13 +933,13 @@
         <v>3</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3" s="7">
         <v>1</v>
@@ -954,7 +954,7 @@
     </row>
     <row r="4" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" s="7">
         <v>0.75</v>
@@ -964,14 +964,14 @@
         <v>0</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" s="8">
         <v>0</v>
@@ -986,7 +986,7 @@
     </row>
     <row r="6" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" s="8">
         <v>0.75</v>
@@ -996,14 +996,14 @@
         <v>0</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7" s="8">
         <v>0</v>
@@ -1018,7 +1018,7 @@
     </row>
     <row r="8" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C8" s="8">
         <v>0</v>
@@ -1033,7 +1033,7 @@
     </row>
     <row r="9" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9" s="8">
         <v>0.75</v>
@@ -1043,7 +1043,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -1186,7 +1186,7 @@
   </sheetPr>
   <dimension ref="B1:H21"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -1214,13 +1214,13 @@
     </row>
     <row r="2" spans="2:8" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>1</v>
@@ -1232,12 +1232,12 @@
         <v>3</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C3" s="18">
         <v>1</v>
@@ -1254,12 +1254,12 @@
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" s="18">
         <v>2</v>
@@ -1276,12 +1276,12 @@
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5" s="18">
         <v>3</v>
@@ -1298,12 +1298,12 @@
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C6" s="19">
         <v>4</v>
@@ -1319,7 +1319,7 @@
     </row>
     <row r="7" spans="2:8" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C7" s="19">
         <v>5</v>
@@ -1335,7 +1335,7 @@
     </row>
     <row r="8" spans="2:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C8" s="19">
         <v>6</v>
@@ -1351,7 +1351,7 @@
     </row>
     <row r="9" spans="2:8" ht="43" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C9" s="19">
         <v>7</v>
@@ -1367,7 +1367,7 @@
     </row>
     <row r="10" spans="2:8" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" s="19">
         <v>8</v>
@@ -1383,7 +1383,7 @@
     </row>
     <row r="11" spans="2:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C11" s="19">
         <v>9</v>
@@ -1399,7 +1399,7 @@
     </row>
     <row r="12" spans="2:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C12" s="19">
         <v>10</v>
@@ -1415,7 +1415,7 @@
     </row>
     <row r="13" spans="2:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C13" s="19">
         <v>11</v>
@@ -1431,7 +1431,7 @@
     </row>
     <row r="14" spans="2:8" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C14" s="19">
         <v>12</v>
@@ -1447,7 +1447,7 @@
     </row>
     <row r="15" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C15" s="19">
         <v>13</v>
@@ -1463,7 +1463,7 @@
     </row>
     <row r="16" spans="2:8" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C16" s="21">
         <v>14</v>
@@ -1479,7 +1479,7 @@
     </row>
     <row r="17" spans="2:8" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C17" s="21">
         <v>15</v>
@@ -1496,12 +1496,12 @@
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C18" s="21">
         <v>16</v>
@@ -1517,7 +1517,7 @@
     </row>
     <row r="19" spans="2:8" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C19" s="21">
         <v>17</v>
@@ -1533,7 +1533,7 @@
     </row>
     <row r="20" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C20" s="21">
         <v>18</v>
@@ -1550,12 +1550,12 @@
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C21" s="21">
         <v>19</v>
@@ -1572,7 +1572,7 @@
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1687,7 +1687,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>1</v>
@@ -1699,7 +1699,7 @@
         <v>3</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1717,10 +1717,10 @@
         <v>0</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1738,10 +1738,10 @@
         <v>0</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1760,7 +1760,7 @@
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1941,7 +1941,7 @@
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1987,10 +1987,10 @@
         <v>0</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2008,10 +2008,10 @@
         <v>0</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2096,8 +2096,8 @@
   </sheetPr>
   <dimension ref="B1:G13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2153,7 +2153,7 @@
     </row>
     <row r="4" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="7">
         <v>1</v>
@@ -2168,7 +2168,7 @@
     </row>
     <row r="5" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="8">
         <v>1</v>
@@ -2183,23 +2183,26 @@
     </row>
     <row r="6" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="C6" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="9">
         <f>--(Table145[[#This Row],[% COMPLETE]]&gt;=1)</f>
-        <v>0</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>11</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E6" s="2"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="8"/>
+      <c r="B7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0</v>
+      </c>
       <c r="D7" s="9">
         <f>--(Table145[[#This Row],[% COMPLETE]]&gt;=1)</f>
         <v>0</v>

</xml_diff>

<commit_message>
Updated Progress Report & SRS
</commit_message>
<xml_diff>
--- a/Progress-Report.xlsx
+++ b/Progress-Report.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26408"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/megavancena/HOM-Documents/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6820" yWindow="500" windowWidth="23860" windowHeight="17540"/>
+    <workbookView xWindow="17085" yWindow="465" windowWidth="19440" windowHeight="13740" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="User Interface" sheetId="5" r:id="rId1"/>
@@ -23,12 +18,12 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'Test Cases'!$2:$2</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'User Interface'!$2:$2</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -36,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
   <si>
     <t>DONE</t>
   </si>
@@ -177,12 +172,6 @@
   </si>
   <si>
     <t>ITERATION</t>
-  </si>
-  <si>
-    <t>Not yet done testing</t>
-  </si>
-  <si>
-    <t>Still to test</t>
   </si>
   <si>
     <t xml:space="preserve">Iteration 1 Class Diagram </t>
@@ -195,7 +184,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="13"/>
       <color theme="4" tint="0.39991454817346722"/>
@@ -881,7 +870,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -895,23 +884,23 @@
   </sheetPr>
   <dimension ref="B1:G29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.1" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="2.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="2" customWidth="1"/>
-    <col min="3" max="4" width="14.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="37.42578125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="2.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="14.6640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="37.44140625" style="8" customWidth="1"/>
     <col min="6" max="6" width="19" style="4" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.7109375" style="1"/>
+    <col min="7" max="7" width="16.5546875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:7" s="10" customFormat="1" ht="21.95" customHeight="1">
       <c r="B1" s="11" t="s">
         <v>2</v>
       </c>
@@ -919,7 +908,7 @@
       <c r="D1" s="12"/>
       <c r="E1" s="13"/>
     </row>
-    <row r="2" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:7" ht="21.95" customHeight="1">
       <c r="B2" s="14" t="s">
         <v>5</v>
       </c>
@@ -937,7 +926,7 @@
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:7" ht="21.95" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
@@ -952,7 +941,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:7" ht="21.95" customHeight="1">
       <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
@@ -969,7 +958,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:7" ht="21.95" customHeight="1">
       <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
@@ -984,7 +973,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:7" ht="21.95" customHeight="1">
       <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
@@ -1001,7 +990,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7" ht="21.95" customHeight="1">
       <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
@@ -1016,7 +1005,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7" ht="21.95" customHeight="1">
       <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
@@ -1031,7 +1020,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:7" ht="21.95" customHeight="1">
       <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1048,7 +1037,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:7" ht="21.95" customHeight="1">
       <c r="C10" s="8"/>
       <c r="D10" s="9">
         <f>--(Table14[[#This Row],[% COMPLETE]]&gt;=1)</f>
@@ -1058,7 +1047,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:7" ht="21.95" customHeight="1">
       <c r="C11" s="8"/>
       <c r="D11" s="9">
         <f>--(Table14[[#This Row],[% COMPLETE]]&gt;=1)</f>
@@ -1068,7 +1057,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:7" ht="21.95" customHeight="1">
       <c r="C12" s="8"/>
       <c r="D12" s="9">
         <f>--(Table14[[#This Row],[% COMPLETE]]&gt;=1)</f>
@@ -1078,7 +1067,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:7" ht="21.95" customHeight="1">
       <c r="C13" s="8"/>
       <c r="D13" s="9">
         <f>--(Table14[[#This Row],[% COMPLETE]]&gt;=1)</f>
@@ -1088,22 +1077,22 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="2:7" ht="21.95" customHeight="1"/>
+    <row r="15" spans="2:7" ht="21.95" customHeight="1"/>
+    <row r="16" spans="2:7" ht="21.95" customHeight="1"/>
+    <row r="17" ht="21.95" customHeight="1"/>
+    <row r="18" ht="21.95" customHeight="1"/>
+    <row r="19" ht="21.95" customHeight="1"/>
+    <row r="20" ht="21.95" customHeight="1"/>
+    <row r="21" ht="21.95" customHeight="1"/>
+    <row r="22" ht="21.95" customHeight="1"/>
+    <row r="23" ht="21.95" customHeight="1"/>
+    <row r="24" ht="21.95" customHeight="1"/>
+    <row r="25" ht="21.95" customHeight="1"/>
+    <row r="26" ht="21.95" customHeight="1"/>
+    <row r="27" ht="21.95" customHeight="1"/>
+    <row r="28" ht="21.95" customHeight="1"/>
+    <row r="29" ht="21.95" customHeight="1"/>
   </sheetData>
   <conditionalFormatting sqref="C3:C13">
     <cfRule type="dataBar" priority="1">
@@ -1186,25 +1175,25 @@
   </sheetPr>
   <dimension ref="B1:H21"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView showGridLines="0" topLeftCell="A11" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="33" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="2.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="2.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" style="3" customWidth="1"/>
     <col min="4" max="4" width="9" style="3" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" style="8" customWidth="1"/>
     <col min="6" max="6" width="7" style="4" customWidth="1"/>
-    <col min="7" max="7" width="32.85546875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.7109375" style="1"/>
+    <col min="7" max="7" width="32.88671875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:8" s="10" customFormat="1" ht="21.95" customHeight="1">
       <c r="B1" s="11" t="s">
         <v>2</v>
       </c>
@@ -1212,7 +1201,7 @@
       <c r="D1" s="12"/>
       <c r="E1" s="13"/>
     </row>
-    <row r="2" spans="2:8" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:8" ht="21.95" customHeight="1">
       <c r="B2" s="20" t="s">
         <v>18</v>
       </c>
@@ -1235,7 +1224,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:8" ht="21.95" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
@@ -1257,7 +1246,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:8" ht="21.95" customHeight="1">
       <c r="B4" s="5" t="s">
         <v>21</v>
       </c>
@@ -1279,7 +1268,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:8" ht="21.95" customHeight="1">
       <c r="B5" s="5" t="s">
         <v>23</v>
       </c>
@@ -1301,7 +1290,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:8" ht="36" customHeight="1">
       <c r="B6" s="2" t="s">
         <v>26</v>
       </c>
@@ -1317,7 +1306,7 @@
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="2:8" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:8" ht="21.95" customHeight="1">
       <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
@@ -1333,7 +1322,7 @@
       </c>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="2:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:8" ht="33.950000000000003" customHeight="1">
       <c r="B8" s="2" t="s">
         <v>27</v>
       </c>
@@ -1349,7 +1338,7 @@
       </c>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="2:8" ht="43" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:8" ht="42.95" customHeight="1">
       <c r="B9" s="2" t="s">
         <v>37</v>
       </c>
@@ -1365,7 +1354,7 @@
       </c>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="2:8" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:8" ht="36.950000000000003" customHeight="1">
       <c r="B10" s="2" t="s">
         <v>25</v>
       </c>
@@ -1381,7 +1370,7 @@
       </c>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="2:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:8" ht="39.950000000000003" customHeight="1">
       <c r="B11" s="2" t="s">
         <v>28</v>
       </c>
@@ -1397,7 +1386,7 @@
       </c>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="2:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:8" ht="39.950000000000003" customHeight="1">
       <c r="B12" s="2" t="s">
         <v>38</v>
       </c>
@@ -1413,7 +1402,7 @@
       </c>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="2:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:8" ht="35.1" customHeight="1">
       <c r="B13" s="2" t="s">
         <v>29</v>
       </c>
@@ -1429,7 +1418,7 @@
       </c>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="2:8" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:8" ht="38.1" customHeight="1">
       <c r="B14" s="2" t="s">
         <v>30</v>
       </c>
@@ -1445,7 +1434,7 @@
       </c>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:8" ht="33" customHeight="1">
       <c r="B15" s="2" t="s">
         <v>31</v>
       </c>
@@ -1461,7 +1450,7 @@
       </c>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="2:8" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:8" ht="50.1" customHeight="1">
       <c r="B16" s="2" t="s">
         <v>32</v>
       </c>
@@ -1477,7 +1466,7 @@
       </c>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="2:8" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" ht="30.95" customHeight="1">
       <c r="B17" s="2" t="s">
         <v>33</v>
       </c>
@@ -1499,7 +1488,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" ht="33" customHeight="1">
       <c r="B18" s="2" t="s">
         <v>34</v>
       </c>
@@ -1515,7 +1504,7 @@
       </c>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="2:8" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8" ht="48" customHeight="1">
       <c r="B19" s="2" t="s">
         <v>35</v>
       </c>
@@ -1531,7 +1520,7 @@
       </c>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:8" ht="33" customHeight="1">
       <c r="B20" s="2" t="s">
         <v>20</v>
       </c>
@@ -1553,7 +1542,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8" ht="33" customHeight="1">
       <c r="B21" s="2" t="s">
         <v>36</v>
       </c>
@@ -1657,24 +1646,24 @@
   </sheetPr>
   <dimension ref="B1:G21"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="33" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="2.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="2.42578125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="2.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="6.5546875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="18.5546875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="2.44140625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:7" s="10" customFormat="1" ht="21.95" customHeight="1">
       <c r="B1" s="11" t="s">
         <v>2</v>
       </c>
@@ -1682,7 +1671,7 @@
       <c r="D1" s="12"/>
       <c r="E1" s="13"/>
     </row>
-    <row r="2" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:7" ht="21.95" customHeight="1">
       <c r="B2" s="14" t="s">
         <v>4</v>
       </c>
@@ -1702,7 +1691,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:7" ht="21.95" customHeight="1">
       <c r="B3" s="18">
         <v>1</v>
       </c>
@@ -1710,20 +1699,18 @@
         <v>1</v>
       </c>
       <c r="D3" s="7">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E3" s="6">
         <f>--(Table13[[#This Row],[% COMPLETE]]&gt;=1)</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>48</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F3" s="5"/>
       <c r="G3" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:7" ht="21.95" customHeight="1">
       <c r="B4" s="18">
         <v>2</v>
       </c>
@@ -1731,20 +1718,18 @@
         <v>1</v>
       </c>
       <c r="D4" s="7">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="E4" s="6">
         <f>--(Table13[[#This Row],[% COMPLETE]]&gt;=1)</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>47</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F4" s="5"/>
       <c r="G4" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:7" ht="21.95" customHeight="1">
       <c r="B5" s="18">
         <v>3</v>
       </c>
@@ -1752,18 +1737,18 @@
         <v>1</v>
       </c>
       <c r="D5" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="9">
         <f>--(Table13[[#This Row],[% COMPLETE]]&gt;=1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:7" ht="21.95" customHeight="1">
       <c r="B6" s="19">
         <v>4</v>
       </c>
@@ -1778,7 +1763,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7" ht="21.95" customHeight="1">
       <c r="B7" s="19">
         <v>5</v>
       </c>
@@ -1793,7 +1778,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7" ht="21.95" customHeight="1">
       <c r="B8" s="19">
         <v>6</v>
       </c>
@@ -1808,7 +1793,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:7" ht="21.95" customHeight="1">
       <c r="B9" s="19">
         <v>7</v>
       </c>
@@ -1823,7 +1808,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:7" ht="21.95" customHeight="1">
       <c r="B10" s="19">
         <v>8</v>
       </c>
@@ -1838,7 +1823,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:7" ht="21.95" customHeight="1">
       <c r="B11" s="19">
         <v>9</v>
       </c>
@@ -1853,7 +1838,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:7" ht="21.95" customHeight="1">
       <c r="B12" s="19">
         <v>10</v>
       </c>
@@ -1868,7 +1853,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:7" ht="21.95" customHeight="1">
       <c r="B13" s="19">
         <v>11</v>
       </c>
@@ -1883,7 +1868,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:7" ht="21.95" customHeight="1">
       <c r="B14" s="19">
         <v>12</v>
       </c>
@@ -1897,7 +1882,7 @@
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:7" ht="21.95" customHeight="1">
       <c r="B15" s="19">
         <v>13</v>
       </c>
@@ -1911,7 +1896,7 @@
       </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:7" ht="21.95" customHeight="1">
       <c r="B16" s="19">
         <v>14</v>
       </c>
@@ -1925,7 +1910,7 @@
       </c>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7" ht="21.95" customHeight="1">
       <c r="B17" s="19">
         <v>15</v>
       </c>
@@ -1933,18 +1918,18 @@
         <v>1</v>
       </c>
       <c r="D17" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="17">
         <f>--(Table13[[#This Row],[% COMPLETE]]&gt;=1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7" ht="21.95" customHeight="1">
       <c r="B18" s="19">
         <v>16</v>
       </c>
@@ -1958,7 +1943,7 @@
       </c>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7" ht="21.95" customHeight="1">
       <c r="B19" s="19">
         <v>17</v>
       </c>
@@ -1972,7 +1957,7 @@
       </c>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:7" ht="21.95" customHeight="1">
       <c r="B20" s="19">
         <v>18</v>
       </c>
@@ -1980,20 +1965,18 @@
         <v>1</v>
       </c>
       <c r="D20" s="22">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E20" s="17">
         <f>--(Table13[[#This Row],[% COMPLETE]]&gt;=1)</f>
-        <v>0</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>48</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F20" s="2"/>
       <c r="G20" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:7" ht="21.95" customHeight="1">
       <c r="B21" s="19">
         <v>19</v>
       </c>
@@ -2001,15 +1984,13 @@
         <v>1</v>
       </c>
       <c r="D21" s="22">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E21" s="17">
         <f>--(Table13[[#This Row],[% COMPLETE]]&gt;=1)</f>
-        <v>0</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>48</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F21" s="2"/>
       <c r="G21" s="4" t="s">
         <v>45</v>
       </c>
@@ -2100,19 +2081,19 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="33" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="2.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" style="2" customWidth="1"/>
-    <col min="3" max="4" width="14.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="39.140625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="24.140625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="2.42578125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="2.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" style="2" customWidth="1"/>
+    <col min="3" max="4" width="14.6640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="39.109375" style="8" customWidth="1"/>
+    <col min="6" max="6" width="18.5546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="24.109375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="2.44140625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:7" s="10" customFormat="1" ht="21.95" customHeight="1">
       <c r="B1" s="11" t="s">
         <v>2</v>
       </c>
@@ -2120,7 +2101,7 @@
       <c r="D1" s="12"/>
       <c r="E1" s="13"/>
     </row>
-    <row r="2" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:7" ht="21.95" customHeight="1">
       <c r="B2" s="14" t="s">
         <v>6</v>
       </c>
@@ -2136,7 +2117,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:7" ht="21.95" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
@@ -2151,7 +2132,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:7" ht="21.95" customHeight="1">
       <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
@@ -2166,7 +2147,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:7" ht="21.95" customHeight="1">
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
@@ -2181,9 +2162,9 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:7" ht="21.95" customHeight="1">
       <c r="B6" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C6" s="8">
         <v>1</v>
@@ -2196,9 +2177,9 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7" ht="21.95" customHeight="1">
       <c r="B7" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C7" s="8">
         <v>0</v>
@@ -2211,7 +2192,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7" ht="21.95" customHeight="1">
       <c r="C8" s="8"/>
       <c r="D8" s="9">
         <f>--(Table145[[#This Row],[% COMPLETE]]&gt;=1)</f>
@@ -2221,7 +2202,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:7" ht="21.95" customHeight="1">
       <c r="C9" s="8"/>
       <c r="D9" s="9">
         <f>--(Table145[[#This Row],[% COMPLETE]]&gt;=1)</f>
@@ -2231,7 +2212,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:7" ht="21.95" customHeight="1">
       <c r="C10" s="8"/>
       <c r="D10" s="9">
         <f>--(Table145[[#This Row],[% COMPLETE]]&gt;=1)</f>
@@ -2241,7 +2222,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:7" ht="21.95" customHeight="1">
       <c r="C11" s="8"/>
       <c r="D11" s="9">
         <f>--(Table145[[#This Row],[% COMPLETE]]&gt;=1)</f>
@@ -2251,7 +2232,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:7" ht="21.95" customHeight="1">
       <c r="C12" s="8"/>
       <c r="D12" s="9">
         <f>--(Table145[[#This Row],[% COMPLETE]]&gt;=1)</f>
@@ -2261,7 +2242,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:7" ht="21.95" customHeight="1">
       <c r="C13" s="8"/>
       <c r="D13" s="9">
         <f>--(Table145[[#This Row],[% COMPLETE]]&gt;=1)</f>

</xml_diff>

<commit_message>
Uploaded most recent test cases & updated progress report
</commit_message>
<xml_diff>
--- a/Progress-Report.xlsx
+++ b/Progress-Report.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26408"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/megavancena/HOM-Documents/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17085" yWindow="465" windowWidth="19440" windowHeight="13740" activeTab="2"/>
+    <workbookView xWindow="2980" yWindow="460" windowWidth="23800" windowHeight="17920" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="User Interface" sheetId="5" r:id="rId1"/>
@@ -18,12 +23,12 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'Test Cases'!$2:$2</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'User Interface'!$2:$2</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="55">
   <si>
     <t>DONE</t>
   </si>
@@ -178,13 +183,31 @@
   </si>
   <si>
     <t xml:space="preserve">Iteration 2 Class Diagram </t>
+  </si>
+  <si>
+    <t>No functionality</t>
+  </si>
+  <si>
+    <t>Ask Miguel / Daniel?, Fix layout, match design with other pages</t>
+  </si>
+  <si>
+    <t>Daniel Garcia</t>
+  </si>
+  <si>
+    <t>Kenywil Tiu</t>
+  </si>
+  <si>
+    <t>Margaret Avancena</t>
+  </si>
+  <si>
+    <t>Rheygine Medel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="13"/>
       <color theme="4" tint="0.39991454817346722"/>
@@ -279,7 +302,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -354,6 +377,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -870,7 +896,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -885,22 +911,22 @@
   <dimension ref="B1:G29"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.1" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" style="2" customWidth="1"/>
-    <col min="3" max="4" width="14.6640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="37.44140625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="2.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" style="2" customWidth="1"/>
+    <col min="3" max="4" width="14.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="37.42578125" style="8" customWidth="1"/>
     <col min="6" max="6" width="19" style="4" customWidth="1"/>
-    <col min="7" max="7" width="16.5546875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="15.5546875" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.6640625" style="1"/>
+    <col min="7" max="7" width="16.5703125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="10" customFormat="1" ht="21.95" customHeight="1">
+    <row r="1" spans="2:7" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="11" t="s">
         <v>2</v>
       </c>
@@ -908,7 +934,7 @@
       <c r="D1" s="12"/>
       <c r="E1" s="13"/>
     </row>
-    <row r="2" spans="2:7" ht="21.95" customHeight="1">
+    <row r="2" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="14" t="s">
         <v>5</v>
       </c>
@@ -926,7 +952,7 @@
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="2:7" ht="21.95" customHeight="1">
+    <row r="3" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
@@ -938,10 +964,12 @@
         <v>1</v>
       </c>
       <c r="E3" s="5"/>
-      <c r="F3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="2:7" ht="21.95" customHeight="1">
+    <row r="4" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
@@ -955,10 +983,12 @@
       <c r="E4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="2:7" ht="21.95" customHeight="1">
+    <row r="5" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
@@ -973,54 +1003,60 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="2:7" ht="21.95" customHeight="1">
+    <row r="6" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="8">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="D6" s="9">
         <f>--(Table14[[#This Row],[% COMPLETE]]&gt;=1)</f>
-        <v>0</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="2:7" ht="21.95" customHeight="1">
+    <row r="7" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="9">
         <f>--(Table14[[#This Row],[% COMPLETE]]&gt;=1)</f>
-        <v>0</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="2:7" ht="21.95" customHeight="1">
+    <row r="8" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="9">
         <f>--(Table14[[#This Row],[% COMPLETE]]&gt;=1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="2"/>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="2:7" ht="21.95" customHeight="1">
+    <row r="9" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1032,12 +1068,14 @@
         <v>0</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="2:7" ht="21.95" customHeight="1">
+    <row r="10" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="8"/>
       <c r="D10" s="9">
         <f>--(Table14[[#This Row],[% COMPLETE]]&gt;=1)</f>
@@ -1047,7 +1085,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="2:7" ht="21.95" customHeight="1">
+    <row r="11" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="8"/>
       <c r="D11" s="9">
         <f>--(Table14[[#This Row],[% COMPLETE]]&gt;=1)</f>
@@ -1057,7 +1095,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="2:7" ht="21.95" customHeight="1">
+    <row r="12" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="8"/>
       <c r="D12" s="9">
         <f>--(Table14[[#This Row],[% COMPLETE]]&gt;=1)</f>
@@ -1067,7 +1105,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="2:7" ht="21.95" customHeight="1">
+    <row r="13" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C13" s="8"/>
       <c r="D13" s="9">
         <f>--(Table14[[#This Row],[% COMPLETE]]&gt;=1)</f>
@@ -1077,22 +1115,22 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="2:7" ht="21.95" customHeight="1"/>
-    <row r="15" spans="2:7" ht="21.95" customHeight="1"/>
-    <row r="16" spans="2:7" ht="21.95" customHeight="1"/>
-    <row r="17" ht="21.95" customHeight="1"/>
-    <row r="18" ht="21.95" customHeight="1"/>
-    <row r="19" ht="21.95" customHeight="1"/>
-    <row r="20" ht="21.95" customHeight="1"/>
-    <row r="21" ht="21.95" customHeight="1"/>
-    <row r="22" ht="21.95" customHeight="1"/>
-    <row r="23" ht="21.95" customHeight="1"/>
-    <row r="24" ht="21.95" customHeight="1"/>
-    <row r="25" ht="21.95" customHeight="1"/>
-    <row r="26" ht="21.95" customHeight="1"/>
-    <row r="27" ht="21.95" customHeight="1"/>
-    <row r="28" ht="21.95" customHeight="1"/>
-    <row r="29" ht="21.95" customHeight="1"/>
+    <row r="14" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <conditionalFormatting sqref="C3:C13">
     <cfRule type="dataBar" priority="1">
@@ -1175,25 +1213,25 @@
   </sheetPr>
   <dimension ref="B1:H21"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A11" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView showGridLines="0" topLeftCell="A8" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14:H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="33" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="2.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="3" customWidth="1"/>
     <col min="4" max="4" width="9" style="3" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="8" customWidth="1"/>
     <col min="6" max="6" width="7" style="4" customWidth="1"/>
-    <col min="7" max="7" width="32.88671875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.6640625" style="1"/>
+    <col min="7" max="7" width="32.85546875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="10" customFormat="1" ht="21.95" customHeight="1">
+    <row r="1" spans="2:8" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="11" t="s">
         <v>2</v>
       </c>
@@ -1201,7 +1239,7 @@
       <c r="D1" s="12"/>
       <c r="E1" s="13"/>
     </row>
-    <row r="2" spans="2:8" ht="21.95" customHeight="1">
+    <row r="2" spans="2:8" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="20" t="s">
         <v>18</v>
       </c>
@@ -1224,7 +1262,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="21.95" customHeight="1">
+    <row r="3" spans="2:8" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
@@ -1246,7 +1284,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="21.95" customHeight="1">
+    <row r="4" spans="2:8" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
         <v>21</v>
       </c>
@@ -1268,7 +1306,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="21.95" customHeight="1">
+    <row r="5" spans="2:8" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="s">
         <v>23</v>
       </c>
@@ -1290,7 +1328,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="36" customHeight="1">
+    <row r="6" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>26</v>
       </c>
@@ -1306,7 +1344,7 @@
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="2:8" ht="21.95" customHeight="1">
+    <row r="7" spans="2:8" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
@@ -1322,7 +1360,7 @@
       </c>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="2:8" ht="33.950000000000003" customHeight="1">
+    <row r="8" spans="2:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>27</v>
       </c>
@@ -1338,7 +1376,7 @@
       </c>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="2:8" ht="42.95" customHeight="1">
+    <row r="9" spans="2:8" ht="43" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>37</v>
       </c>
@@ -1354,7 +1392,7 @@
       </c>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="2:8" ht="36.950000000000003" customHeight="1">
+    <row r="10" spans="2:8" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>25</v>
       </c>
@@ -1370,7 +1408,7 @@
       </c>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="2:8" ht="39.950000000000003" customHeight="1">
+    <row r="11" spans="2:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>28</v>
       </c>
@@ -1386,7 +1424,7 @@
       </c>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="2:8" ht="39.950000000000003" customHeight="1">
+    <row r="12" spans="2:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>38</v>
       </c>
@@ -1396,13 +1434,16 @@
       <c r="D12" s="24">
         <v>2</v>
       </c>
+      <c r="E12" s="8">
+        <v>0</v>
+      </c>
       <c r="F12" s="9">
         <f>--(Table1[[#This Row],[% COMPLETE]]&gt;=1)</f>
         <v>0</v>
       </c>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="2:8" ht="35.1" customHeight="1">
+    <row r="13" spans="2:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>29</v>
       </c>
@@ -1418,7 +1459,7 @@
       </c>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="2:8" ht="38.1" customHeight="1">
+    <row r="14" spans="2:8" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>30</v>
       </c>
@@ -1428,13 +1469,19 @@
       <c r="D14" s="24">
         <v>2</v>
       </c>
+      <c r="E14" s="8">
+        <v>1</v>
+      </c>
       <c r="F14" s="9">
         <f>--(Table1[[#This Row],[% COMPLETE]]&gt;=1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="2:8" ht="33" customHeight="1">
+      <c r="H14" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>31</v>
       </c>
@@ -1444,13 +1491,19 @@
       <c r="D15" s="24">
         <v>2</v>
       </c>
+      <c r="E15" s="8">
+        <v>1</v>
+      </c>
       <c r="F15" s="9">
         <f>--(Table1[[#This Row],[% COMPLETE]]&gt;=1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="2:8" ht="50.1" customHeight="1">
+      <c r="H15" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>32</v>
       </c>
@@ -1460,13 +1513,19 @@
       <c r="D16" s="24">
         <v>2</v>
       </c>
+      <c r="E16" s="8">
+        <v>1</v>
+      </c>
       <c r="F16" s="9">
         <f>--(Table1[[#This Row],[% COMPLETE]]&gt;=1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="2:8" ht="30.95" customHeight="1">
+      <c r="H16" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>33</v>
       </c>
@@ -1488,7 +1547,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="33" customHeight="1">
+    <row r="18" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>34</v>
       </c>
@@ -1504,7 +1563,7 @@
       </c>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="2:8" ht="48" customHeight="1">
+    <row r="19" spans="2:8" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>35</v>
       </c>
@@ -1520,7 +1579,7 @@
       </c>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="2:8" ht="33" customHeight="1">
+    <row r="20" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>20</v>
       </c>
@@ -1542,7 +1601,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="33" customHeight="1">
+    <row r="21" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
         <v>36</v>
       </c>
@@ -1646,24 +1705,24 @@
   </sheetPr>
   <dimension ref="B1:G21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="33" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="6.5546875" style="8" customWidth="1"/>
-    <col min="6" max="6" width="28.33203125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="18.5546875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="2.44140625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.6640625" style="1"/>
+    <col min="1" max="1" width="2.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="2.42578125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="10" customFormat="1" ht="21.95" customHeight="1">
+    <row r="1" spans="2:7" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="11" t="s">
         <v>2</v>
       </c>
@@ -1671,7 +1730,7 @@
       <c r="D1" s="12"/>
       <c r="E1" s="13"/>
     </row>
-    <row r="2" spans="2:7" ht="21.95" customHeight="1">
+    <row r="2" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="14" t="s">
         <v>4</v>
       </c>
@@ -1691,7 +1750,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="21.95" customHeight="1">
+    <row r="3" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="18">
         <v>1</v>
       </c>
@@ -1710,7 +1769,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="21.95" customHeight="1">
+    <row r="4" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="18">
         <v>2</v>
       </c>
@@ -1729,7 +1788,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="21.95" customHeight="1">
+    <row r="5" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="18">
         <v>3</v>
       </c>
@@ -1748,7 +1807,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="21.95" customHeight="1">
+    <row r="6" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="19">
         <v>4</v>
       </c>
@@ -1763,7 +1822,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="2:7" ht="21.95" customHeight="1">
+    <row r="7" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="19">
         <v>5</v>
       </c>
@@ -1778,7 +1837,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="2:7" ht="21.95" customHeight="1">
+    <row r="8" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="19">
         <v>6</v>
       </c>
@@ -1793,7 +1852,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="2:7" ht="21.95" customHeight="1">
+    <row r="9" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="19">
         <v>7</v>
       </c>
@@ -1808,7 +1867,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="2:7" ht="21.95" customHeight="1">
+    <row r="10" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="19">
         <v>8</v>
       </c>
@@ -1823,7 +1882,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="2:7" ht="21.95" customHeight="1">
+    <row r="11" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="19">
         <v>9</v>
       </c>
@@ -1838,7 +1897,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="2:7" ht="21.95" customHeight="1">
+    <row r="12" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="19">
         <v>10</v>
       </c>
@@ -1853,7 +1912,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="2:7" ht="21.95" customHeight="1">
+    <row r="13" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="19">
         <v>11</v>
       </c>
@@ -1868,49 +1927,64 @@
       <c r="F13" s="2"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="2:7" ht="21.95" customHeight="1">
+    <row r="14" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="19">
         <v>12</v>
       </c>
       <c r="C14" s="24">
         <v>2</v>
       </c>
-      <c r="D14" s="16"/>
+      <c r="D14" s="25">
+        <v>1</v>
+      </c>
       <c r="E14" s="17">
         <f>--(Table13[[#This Row],[% COMPLETE]]&gt;=1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="2:7" ht="21.95" customHeight="1">
+      <c r="G14" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="19">
         <v>13</v>
       </c>
       <c r="C15" s="24">
         <v>2</v>
       </c>
-      <c r="D15" s="16"/>
+      <c r="D15" s="25">
+        <v>1</v>
+      </c>
       <c r="E15" s="17">
         <f>--(Table13[[#This Row],[% COMPLETE]]&gt;=1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="2:7" ht="21.95" customHeight="1">
+      <c r="G15" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="19">
         <v>14</v>
       </c>
       <c r="C16" s="24">
         <v>2</v>
       </c>
-      <c r="D16" s="16"/>
+      <c r="D16" s="25">
+        <v>1</v>
+      </c>
       <c r="E16" s="17">
         <f>--(Table13[[#This Row],[% COMPLETE]]&gt;=1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="2:7" ht="21.95" customHeight="1">
+      <c r="G16" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="19">
         <v>15</v>
       </c>
@@ -1929,7 +2003,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="21.95" customHeight="1">
+    <row r="18" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="19">
         <v>16</v>
       </c>
@@ -1943,7 +2017,7 @@
       </c>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:7" ht="21.95" customHeight="1">
+    <row r="19" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="19">
         <v>17</v>
       </c>
@@ -1957,7 +2031,7 @@
       </c>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:7" ht="21.95" customHeight="1">
+    <row r="20" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="19">
         <v>18</v>
       </c>
@@ -1976,7 +2050,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="21.95" customHeight="1">
+    <row r="21" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="19">
         <v>19</v>
       </c>
@@ -2077,23 +2151,23 @@
   </sheetPr>
   <dimension ref="B1:G13"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="33" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" style="2" customWidth="1"/>
-    <col min="3" max="4" width="14.6640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="39.109375" style="8" customWidth="1"/>
-    <col min="6" max="6" width="18.5546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="24.109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="2.44140625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.6640625" style="1"/>
+    <col min="1" max="1" width="2.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="14.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="39.140625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="2.42578125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="10" customFormat="1" ht="21.95" customHeight="1">
+    <row r="1" spans="2:7" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="11" t="s">
         <v>2</v>
       </c>
@@ -2101,7 +2175,7 @@
       <c r="D1" s="12"/>
       <c r="E1" s="13"/>
     </row>
-    <row r="2" spans="2:7" ht="21.95" customHeight="1">
+    <row r="2" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="14" t="s">
         <v>6</v>
       </c>
@@ -2117,7 +2191,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="2:7" ht="21.95" customHeight="1">
+    <row r="3" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
@@ -2132,7 +2206,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="2:7" ht="21.95" customHeight="1">
+    <row r="4" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
@@ -2147,7 +2221,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="2:7" ht="21.95" customHeight="1">
+    <row r="5" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
@@ -2162,7 +2236,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="2:7" ht="21.95" customHeight="1">
+    <row r="6" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>47</v>
       </c>
@@ -2177,7 +2251,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="2:7" ht="21.95" customHeight="1">
+    <row r="7" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>48</v>
       </c>
@@ -2192,7 +2266,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="2:7" ht="21.95" customHeight="1">
+    <row r="8" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="8"/>
       <c r="D8" s="9">
         <f>--(Table145[[#This Row],[% COMPLETE]]&gt;=1)</f>
@@ -2202,7 +2276,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="2:7" ht="21.95" customHeight="1">
+    <row r="9" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="8"/>
       <c r="D9" s="9">
         <f>--(Table145[[#This Row],[% COMPLETE]]&gt;=1)</f>
@@ -2212,7 +2286,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="2:7" ht="21.95" customHeight="1">
+    <row r="10" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="8"/>
       <c r="D10" s="9">
         <f>--(Table145[[#This Row],[% COMPLETE]]&gt;=1)</f>
@@ -2222,7 +2296,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="2:7" ht="21.95" customHeight="1">
+    <row r="11" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="8"/>
       <c r="D11" s="9">
         <f>--(Table145[[#This Row],[% COMPLETE]]&gt;=1)</f>
@@ -2232,7 +2306,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="2:7" ht="21.95" customHeight="1">
+    <row r="12" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="8"/>
       <c r="D12" s="9">
         <f>--(Table145[[#This Row],[% COMPLETE]]&gt;=1)</f>
@@ -2242,7 +2316,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="2:7" ht="21.95" customHeight="1">
+    <row r="13" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C13" s="8"/>
       <c r="D13" s="9">
         <f>--(Table145[[#This Row],[% COMPLETE]]&gt;=1)</f>

</xml_diff>